<commit_message>
Lots of 214 progress, now have a working player
</commit_message>
<xml_diff>
--- a/24-25Year/Fall24/DES214/PCGProject/PCGSubmission/2DTopDownProceduralShooter.xlsx
+++ b/24-25Year/Fall24/DES214/PCGProject/PCGSubmission/2DTopDownProceduralShooter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KingLoui1221\Documents\DIT Stuff\DITRepo\DITWork\24-25Year\Fall24\DES214\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KingLoui1221\Documents\DIT Stuff\DITRepo\DITWork\24-25Year\Fall24\DES214\PCGProject\PCGSubmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A813D5-3EB2-41DE-B916-5D56C7D78A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DACAF39-8F27-489E-A739-2D8FEEB05746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -2405,8 +2405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Enemies and powerups are in
</commit_message>
<xml_diff>
--- a/24-25Year/Fall24/DES214/PCGProject/PCGSubmission/2DTopDownProceduralShooter.xlsx
+++ b/24-25Year/Fall24/DES214/PCGProject/PCGSubmission/2DTopDownProceduralShooter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KingLoui1221\Documents\DIT Stuff\DITRepo\DITWork\24-25Year\Fall24\DES214\PCGProject\PCGSubmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DACAF39-8F27-489E-A739-2D8FEEB05746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE555B8-4A96-4242-A97D-EA7F6904FC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2405,8 +2405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -2736,10 +2736,10 @@
     <row r="29" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
       <c r="A29" s="37">
         <f>IF(LEFT(B29,2)="No",-0.1,IF(LEFT(B29,7)="Partial",0,IF(LEFT(B29,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>37</v>
@@ -2762,10 +2762,10 @@
     <row r="31" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
       <c r="A31" s="38">
         <f>IF(LEFT(B31,2)="No",-0.1,IF(LEFT(B31,7)="Partial",0,IF(LEFT(B31,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>39</v>
@@ -2867,10 +2867,10 @@
     <row r="40" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
       <c r="A40" s="37">
         <f>IF(LEFT(B40,2)="No",-0.1,IF(LEFT(B40,7)="Partial",0,IF(LEFT(B40,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B40" s="40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>44</v>
@@ -2893,10 +2893,10 @@
     <row r="42" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
       <c r="A42" s="38">
         <f>IF(LEFT(B42,2)="No",-0.1,IF(LEFT(B42,7)="Partial",0,IF(LEFT(B42,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B42" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
PCG done and June twine thing
</commit_message>
<xml_diff>
--- a/24-25Year/Fall24/DES214/PCGProject/PCGSubmission/2DTopDownProceduralShooter.xlsx
+++ b/24-25Year/Fall24/DES214/PCGProject/PCGSubmission/2DTopDownProceduralShooter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KingLoui1221\Documents\DIT Stuff\DITRepo\DITWork\24-25Year\Fall24\DES214\PCGProject\PCGSubmission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chaos\Documents\DIT Work\DITRepo\24-25Year\Fall24\DES214\PCGProject\PCGSubmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE555B8-4A96-4242-A97D-EA7F6904FC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E56A94-A17E-45C2-9F0F-162DBB96CFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="133">
   <si>
     <t>PLAYTEST REPORT #1</t>
   </si>
@@ -1263,6 +1263,156 @@
   </si>
   <si>
     <t>This project was super rough. I went into it super ambitious and ready to make my first real project in godot, and do something really cool with it. I then got bronchitis and couldn't work on anything for two and a half weeks. As it is I've gotten the project to the point where I'm almost done with the map itself, it took several retries and lots of iteration but I'm now happy with the way it's generating. All I need to do now is connect my development phases and add the resolution section. In terms of gameplay I have the frameworks for enemies and players but nothing else. I still need to actually create the player and enemies, as well as powerups. Telemetry isn't done but I'm hoping that should be very easy. And obviously since I don't have a game, I can't playtest. Overall I am very, very behind. However, I am still excited about this project and even if I'm not allowed to resubmit or otherwise try for a better score then I will probably try to advance this project. I think that if I'm able to dedicate some more time to it I'll be able to make something genuinely cool. My plan is to make a variety of handmade interesting rooms, along with cool combat and a challenging boss. In terms of the actual technical side of things I started off generating corridors in exactly the way Ellinger said, but eventually decided that I wanted handmade rooms and it would be easier if I placed those first and did the corridors afterwards. So right now the way my algorithm works is that it places the rooms randomly, then uses A* to create a path between all the entrances so I can guarantee that all the rooms are connected. I then branch off of that A* path to create my interesting PCG. I think it's a good system that allows for a lot of flexibilty. It took me a few tries to get to this point but I did it in the end. This of course is after I completed the very fun process of trying to figure out how to place tiles through code in Godot. I like their tilemap system but right now the code side is a little obtuse. That was the first major hurdle, the second was trying to rotate the rooms. For my rooms I'm using something called "patterns" which is essentially a prefab of tiles. Now Godot lets you rotate these while placing them in editor, but there's no way to do that in code. Luckily, Godot is open source. So my friend Ben and I went on the github and found the code which rotated the pattern in editor, then I just made my own function that uses that code. Problem solved and now I could rotate rooms. Since then it has been the usual stream of bugs and iteration to make things work and look good, but I'm happy with where my generation is now. Overall I would say that this was a cool, fun project that I really wish I'd had more time to spend on. It sucked falling behind on this one and I genuinely did try to catch up but I wasn't able to. The cheat codes are "R" to reset, scroll to zoom in and out, and hold middle mouse to pan the camera.</t>
+  </si>
+  <si>
+    <t>Is game too hard, does it take too long, is it fun</t>
+  </si>
+  <si>
+    <t>Lab D Goals Met</t>
+  </si>
+  <si>
+    <t>Smilewire Team Space</t>
+  </si>
+  <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
+    <t>Ryan Peterson, teammate, BAGD, never played</t>
+  </si>
+  <si>
+    <t>Direction observation</t>
+  </si>
+  <si>
+    <t>Ryan felt that the player started off very slow and thinks that the base speed should be higher with the speed powerups giving less of a bonus. There was also a point where he didn't want to pick up any more speed boosts because he was too fast. Ryan was a little confused by the different firing modes, he had trouble knowing what mode he was in, specifically when using the shotgun. Ryan had a lot of issues with navigation, he would frequently double back or just kind of wander around. He also said multiple times that things felt very samey and that it was hard to tell where he was. Ryan did make it to the boss and beat them so fast that he thought something had gone wrong. After the chaos and sheer tension of development 3 the boss felt like a big let down.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clearly speed needs to be adjusted and the speed powerup nerfed. Ryan started to slow and ended up way too fast. Navigation is also an issue, which I expected as every part of the level uses the same tileset. A few positives is that overall the difficulty scaling was good, each development phase felt distinctly different from the last. It was a little trivial because of the sheer quantity of powerups that Ryan was able to pickup, making him way too strong. </t>
+  </si>
+  <si>
+    <t>Overall decrease the amount of powerups by a lot to ensure that the player is not as strong by the end. I'll also probably shrink the size of the level so it doesn't take so long and isn't so hard to get lost in. For now I'll probably just increase the bosses health by quite a bit and see what happens. I'll also increase the players base speed and make the speed powerups not give as much of a boost.</t>
+  </si>
+  <si>
+    <t>Lab E Goals Met</t>
+  </si>
+  <si>
+    <t>Smilewire Teamspace</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>See if previous changes were good, see if level is easier to navigate, see if boss is right difficulty now</t>
+  </si>
+  <si>
+    <t>Krystal Amersbach, teammate, BFA, never played</t>
+  </si>
+  <si>
+    <t>Direct Observation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krystal didn't understand the different firing modes at first as with only two bullets there isn't that much of a difference. She did get it after a few tries however. Krystal had major problems with navigation and more often than not would just move around at random. Krystal also expressed this several times during the playtest, including saying "why does it feel like I've already been here," in reference to both the fact that she was lost and how samey everything looks. Krystal then used the map camera to try to figure out the way forward. There were also still a lot of powerups and Krystal was very powerful by development 2. She started skipping powerups at some point because she was so strong that she didn't need them. The boss was a lot harder but now sees the player too early and starts shooting down the corridor as the player is trying to enter the boss room. </t>
+  </si>
+  <si>
+    <t>Navigation is still a problem even after shrinking the level, which I was half expecting but hoped wouldn't be an issue. There were also still way too many powerups and Krystal got way too strong by the end, the boss took longer to kill but wasn't actually any more difficult, just illusion. There's also a bug with the firing mode cycling which causes the modes to not act as intended, making it hard to determine the distance between the burst and shotgun. Krystal used the map camera without being prompted.</t>
+  </si>
+  <si>
+    <t>I'm going to lean heavier into the map camera for navigation, that way people can use it when they get lost. I'll probably add text telling players how to switch to make it seem more like a game feature. I'll also decrease the powerup spawn rate again because there are still way too many, I also want the amount in corridors to be much lower so the player has to enter more rooms for powerups. I'll try to fix the firing mode bug so it doesn't cause more issues. I'll also lower the bosses view distance so it won't start tracking the player too early.</t>
+  </si>
+  <si>
+    <t>See if map camera helps navigation, see if powerups are at a more reasonable level</t>
+  </si>
+  <si>
+    <t>Nick Munoz-Paez, teammate, BAGD, watched Krystal's playtest</t>
+  </si>
+  <si>
+    <t>Nick entered shotgun mode early on and then never changed because he thought that this was the default. He then talked about how he would much rather have his bullets go exactly where he's aiming instead of the slight spread. He was under the impression that there were only two firing modes, after the playtest he said that "switch" firing modes made it seem like there were only two, binary. Nick was very vocal about thinking the health pickup is a waste because he's already at full health, he does not realize that it increases his max health. Nick attempted to use the map camera to navigate but didn't know that you could pan it and so it wasn't super useful. Nick also avoided picking up the speed powerups because he didn't know what they were doing and so figured they had so little affect they were useless. Nick also needed cover to fight the boss as the boss was actually threatening.</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>PlayerShotsFired</t>
+  </si>
+  <si>
+    <t>BasicEnemyShotsFired</t>
+  </si>
+  <si>
+    <t>CharacterBody2DDamageTaken</t>
+  </si>
+  <si>
+    <t>CharacterBody2D</t>
+  </si>
+  <si>
+    <t>BulletPowerupsGrabbed</t>
+  </si>
+  <si>
+    <t>BurstEnemyShotsFired</t>
+  </si>
+  <si>
+    <t>SpeedPowerupsGrabbed</t>
+  </si>
+  <si>
+    <t>HealthPowerupsGrabbed</t>
+  </si>
+  <si>
+    <t>CharacterBody2DHealed</t>
+  </si>
+  <si>
+    <t>SniperEnemyShotsFired</t>
+  </si>
+  <si>
+    <t>ShotgunEnemyShotsFired</t>
+  </si>
+  <si>
+    <t>MachineGunEnemyShotsFired</t>
+  </si>
+  <si>
+    <t>BounceEnemyShotsFired</t>
+  </si>
+  <si>
+    <t>BossEnemyShotsFired</t>
+  </si>
+  <si>
+    <t>PlayerDistanceTraveled</t>
+  </si>
+  <si>
+    <t>RunTime</t>
+  </si>
+  <si>
+    <t>Having the map camera to help navigate is good, but needs further explanation. The powerups still aren't explained super well, the only one that Nick understood was the bullet one. The boss feels a lot better now and probably won't need too many more tweaks. I don't think the firing modes are actually confusing I think Nick just didn't hit shift a single time after picking the shotgun mode the first time.</t>
+  </si>
+  <si>
+    <t>Add more text to explain how to zoom/pan the map camera so that it can be used for navigation better. Might also shrink the level just a little bit more. Up the amount the speed powerup gives so it's actually noticeable again. Change the text for the firing mode to say "cycle" so it's clear there are more than two. Move the boss back a slight bit and maybe add some walls into his arena for us as cover.</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>Are powerups finally fine, is navigation good, is boss fun and challenging</t>
+  </si>
+  <si>
+    <t>June Endstrasser, teammate and TA, BSCSGD, saw a while ago but not recently</t>
+  </si>
+  <si>
+    <t>Direct observation</t>
+  </si>
+  <si>
+    <t>June was able to give feedback directly as a TA, which was greatly appreciated. June liked the overall difficulty progression but had some trouble telling what development phase she was in at first. June believed that the speed powerups actually lessened the spread of bullets in the spread and shotgun modes. June had an easier time navigating as she was able to use the map camera to see where she was. June also gave feedback on requirements specific things, such as having enemies leave a "corpse" behind and differentiating the different development phases with colors. The boss was decently hard but June was able to get it stuck on a wall and after that it wasn't a challenge.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall the game looks a lot better. Navigation is mostly fixed, same with powerups. There's still a little confusion but aside from straight up using text to explain things there's not a whole lot I can do about it. The firing modes work a lot better now and are super cool. The boss is in a good state, just a little too easy to cheese. </t>
+  </si>
+  <si>
+    <t>Add various things that are required, such as the corpses and colors. Make the boss smaller and faster so it isn't as prone to getting stuck. I'll probably add a gradient behind the entire level which transitions from color to color to differentiate different areas. I'll also tweak a few more values like the speed powerup but overall the game is in a good state and is ready for submission.</t>
+  </si>
+  <si>
+    <t>Post mortem 2</t>
+  </si>
+  <si>
+    <t>I'm a lot happier with where my project is at. I didn't expect it to take nearly this long to complete but it is finally done which I'm glad for. I haven't noticed any bugs in my generation for quite a while now which is awesome. I'm also happy that I got at least some kind of gimmick in through the different firing modes. Overall I think the best part of this project was that it gave me a chance to learn the godot game engine and practice using composition via nodes. I'm very happy with how my architecture turned out and I think it will help me a lot in any future godot projects. Overall I faced a lot of setbacks and obviously spent way too long on this project but I'm happy with how it turned out and I'm very glad that I stuck with it.</t>
   </si>
 </sst>
 </file>
@@ -1620,7 +1770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1758,6 +1908,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2405,24 +2558,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="130.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.5546875" style="30" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="130.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="24" thickBot="1">
       <c r="A1" s="46">
         <f>MIN(1,(MAX(0,(SUM(A4:A1004)+IF(ISBLANK(A2),0,MIN(0,A2-0.6)))*IF(A50&lt;&gt;"n/a",1,IF(A39&lt;&gt;"n/a",1.25,IF(A28&lt;&gt;"n/a",5/3,IF(A17&lt;&gt;"n/a",2.5,5))))+IF(A61&lt;&gt;"n/a",0,0.1)+IF(A6&lt;&gt;"n/a",0,-0.1))))</f>
-        <v>0</v>
+        <v>0.88000000000000045</v>
       </c>
       <c r="B1" s="47" t="s">
         <v>74</v>
@@ -2432,7 +2585,7 @@
       </c>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:5" ht="48" thickBot="1">
+    <row r="2" spans="1:5" ht="47.4" thickBot="1">
       <c r="A2" s="45"/>
       <c r="B2" s="44" t="s">
         <v>72</v>
@@ -2441,26 +2594,26 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="4.1500000000000004" customHeight="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="57" t="s">
+    <row r="3" spans="1:5" ht="4.2" customHeight="1">
+      <c r="A3" s="55"/>
+      <c r="B3" s="58" t="s">
         <v>73</v>
       </c>
       <c r="C3" s="35"/>
     </row>
     <row r="4" spans="1:5" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A4" s="55"/>
-      <c r="B4" s="58"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="35" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
-      <c r="A5" s="56"/>
-      <c r="B5" s="59"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="60"/>
       <c r="C5" s="27"/>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A6" s="37">
         <f>IF(LEFT(B6,2)="No",0,IF(LEFT(B6,7)="Partial",0.02,IF(LEFT(B6,4)="Full",0.04,"n/a")))</f>
         <v>0.04</v>
@@ -2473,7 +2626,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A7" s="37">
         <f>IF(LEFT(B7,2)="No",-0.1,IF(LEFT(B7,7)="Partial",0,IF(LEFT(B7,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2486,7 +2639,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A8" s="38">
         <f>IF(LEFT(B8,2)="No",-0.1,IF(LEFT(B8,7)="Partial",0,IF(LEFT(B8,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2499,7 +2652,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A9" s="38">
         <f>IF(LEFT(B9,2)="No",-0.1,IF(LEFT(B9,7)="Partial",0,IF(LEFT(B9,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2512,7 +2665,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="10" spans="1:5" s="3" customFormat="1">
       <c r="A10" s="38">
         <f>IF(LEFT(B10,2)="No",-0.1,IF(LEFT(B10,7)="Partial",0,IF(LEFT(B10,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2525,7 +2678,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="31.8" thickBot="1">
       <c r="A11" s="39">
         <f>IF(LEFT(B11,2)="No",-0.1,IF(LEFT(B11,7)="Partial",0,IF(LEFT(B11,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2538,7 +2691,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="12" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1">
       <c r="A12" s="38">
         <f>IF(LEFT(B12,2)="No",0,IF(LEFT(B12,7)="Partial",0.01,IF(LEFT(B12,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2551,7 +2704,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="13" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1">
       <c r="A13" s="38">
         <f>IF(LEFT(B13,2)="No",0,IF(LEFT(B13,7)="Partial",0.01,IF(LEFT(B13,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2564,7 +2717,7 @@
       </c>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="14" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1">
       <c r="A14" s="38" t="str">
         <f>IF(LEFT(B14,2)="No",0,IF(LEFT(B14,7)="Partial",0.01,IF(LEFT(B14,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2575,7 +2728,7 @@
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A15" s="39" t="str">
         <f>IF(LEFT(B15,2)="No",0,IF(LEFT(B15,7)="Partial",0.01,IF(LEFT(B15,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2589,7 +2742,7 @@
     <row r="16" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
       <c r="C16" s="27"/>
     </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="17" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A17" s="36">
         <f>IF(LEFT(B17,2)="No",0,IF(LEFT(B17,7)="Partial",0.02,IF(LEFT(B17,4)="Full",0.04,"n/a")))</f>
         <v>0.04</v>
@@ -2602,7 +2755,7 @@
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="18" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A18" s="38">
         <f>IF(LEFT(B18,2)="No",-0.1,IF(LEFT(B18,7)="Partial",0,IF(LEFT(B18,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2615,7 +2768,7 @@
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="19" spans="1:5" s="3" customFormat="1">
       <c r="A19" s="38">
         <f>IF(LEFT(B19,2)="No",-0.1,IF(LEFT(B19,7)="Partial",0,IF(LEFT(B19,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2628,7 +2781,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="20" spans="1:5" s="3" customFormat="1">
       <c r="A20" s="38">
         <f>IF(LEFT(B20,2)="No",-0.1,IF(LEFT(B20,7)="Partial",0,IF(LEFT(B20,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2641,7 +2794,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="21" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A21" s="38">
         <f>IF(LEFT(B21,2)="No",-0.1,IF(LEFT(B21,7)="Partial",0,IF(LEFT(B21,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2654,7 +2807,7 @@
       </c>
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="22" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A22" s="38">
         <f>IF(LEFT(B22,2)="No",-0.1,IF(LEFT(B22,7)="Partial",0,IF(LEFT(B22,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2667,7 +2820,7 @@
       </c>
       <c r="E22" s="25"/>
     </row>
-    <row r="23" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="23" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A23" s="37">
         <f>IF(LEFT(B23,2)="No",0,IF(LEFT(B23,7)="Partial",0.01,IF(LEFT(B23,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2680,7 +2833,7 @@
       </c>
       <c r="E23" s="25"/>
     </row>
-    <row r="24" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="24" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A24" s="38">
         <f>IF(LEFT(B24,2)="No",0,IF(LEFT(B24,7)="Partial",0.01,IF(LEFT(B24,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2693,7 +2846,7 @@
       </c>
       <c r="E24" s="25"/>
     </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="25" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A25" s="38">
         <f>IF(LEFT(B25,2)="No",0,IF(LEFT(B25,7)="Partial",0.01,IF(LEFT(B25,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2706,7 +2859,7 @@
       </c>
       <c r="E25" s="25"/>
     </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="26" spans="1:5" s="3" customFormat="1" ht="16.2" thickBot="1">
       <c r="A26" s="39" t="str">
         <f>IF(LEFT(B26,2)="No",0,IF(LEFT(B26,7)="Partial",0.01,IF(LEFT(B26,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2720,7 +2873,7 @@
     <row r="27" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="28" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A28" s="36">
         <f>IF(LEFT(B28,2)="No",0,IF(LEFT(B28,7)="Partial",0.02,IF(LEFT(B28,4)="Full",0.04,"n/a")))</f>
         <v>0.02</v>
@@ -2733,7 +2886,7 @@
       </c>
       <c r="E28" s="25"/>
     </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="29" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A29" s="37">
         <f>IF(LEFT(B29,2)="No",-0.1,IF(LEFT(B29,7)="Partial",0,IF(LEFT(B29,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2746,20 +2899,20 @@
       </c>
       <c r="E29" s="25"/>
     </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A30" s="38">
         <f>IF(LEFT(B30,2)="No",-0.1,IF(LEFT(B30,7)="Partial",0,IF(LEFT(B30,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="24"/>
     </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A31" s="38">
         <f>IF(LEFT(B31,2)="No",-0.1,IF(LEFT(B31,7)="Partial",0,IF(LEFT(B31,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2772,33 +2925,33 @@
       </c>
       <c r="E31" s="24"/>
     </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="32" spans="1:5" s="3" customFormat="1">
       <c r="A32" s="38">
         <f>IF(LEFT(B32,2)="No",-0.1,IF(LEFT(B32,7)="Partial",0,IF(LEFT(B32,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="24"/>
     </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="33" spans="1:5" s="3" customFormat="1" ht="31.8" thickBot="1">
       <c r="A33" s="39">
         <f>IF(LEFT(B33,2)="No",-0.1,IF(LEFT(B33,7)="Partial",0,IF(LEFT(B33,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E33" s="25"/>
     </row>
-    <row r="34" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="34" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A34" s="38">
         <f>IF(LEFT(B34,2)="No",0,IF(LEFT(B34,7)="Partial",0.01,IF(LEFT(B34,4)="Full",0.02,"n/a")))</f>
         <v>0</v>
@@ -2811,7 +2964,7 @@
       </c>
       <c r="E34" s="25"/>
     </row>
-    <row r="35" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="35" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A35" s="38">
         <f>IF(LEFT(B35,2)="No",0,IF(LEFT(B35,7)="Partial",0.01,IF(LEFT(B35,4)="Full",0.02,"n/a")))</f>
         <v>0</v>
@@ -2824,7 +2977,7 @@
       </c>
       <c r="E35" s="25"/>
     </row>
-    <row r="36" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="36" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A36" s="38">
         <f>IF(LEFT(B36,2)="No",0,IF(LEFT(B36,7)="Partial",0.01,IF(LEFT(B36,4)="Full",0.02,"n/a")))</f>
         <v>0</v>
@@ -2837,7 +2990,7 @@
       </c>
       <c r="E36" s="25"/>
     </row>
-    <row r="37" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="37" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A37" s="39" t="str">
         <f>IF(LEFT(B37,2)="No",0,IF(LEFT(B37,7)="Partial",0.01,IF(LEFT(B37,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2851,7 +3004,7 @@
     <row r="38" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
       <c r="C38" s="27"/>
     </row>
-    <row r="39" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="39" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A39" s="36">
         <f>IF(LEFT(B39,2)="No",0,IF(LEFT(B39,7)="Partial",0.02,IF(LEFT(B39,4)="Full",0.04,"n/a")))</f>
         <v>0</v>
@@ -2864,7 +3017,7 @@
       </c>
       <c r="E39" s="24"/>
     </row>
-    <row r="40" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="40" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A40" s="37">
         <f>IF(LEFT(B40,2)="No",-0.1,IF(LEFT(B40,7)="Partial",0,IF(LEFT(B40,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2877,7 +3030,7 @@
       </c>
       <c r="E40" s="25"/>
     </row>
-    <row r="41" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="41" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A41" s="38">
         <f>IF(LEFT(B41,2)="No",-0.1,IF(LEFT(B41,7)="Partial",0,IF(LEFT(B41,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2890,7 +3043,7 @@
       </c>
       <c r="E41" s="24"/>
     </row>
-    <row r="42" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="42" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A42" s="38">
         <f>IF(LEFT(B42,2)="No",-0.1,IF(LEFT(B42,7)="Partial",0,IF(LEFT(B42,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2903,33 +3056,33 @@
       </c>
       <c r="E42" s="24"/>
     </row>
-    <row r="43" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="43" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A43" s="38">
         <f>IF(LEFT(B43,2)="No",-0.1,IF(LEFT(B43,7)="Partial",0,IF(LEFT(B43,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B43" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E43" s="24"/>
     </row>
-    <row r="44" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="44" spans="1:5" s="3" customFormat="1" ht="31.8" thickBot="1">
       <c r="A44" s="39">
         <f>IF(LEFT(B44,2)="No",-0.1,IF(LEFT(B44,7)="Partial",0,IF(LEFT(B44,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B44" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E44" s="25"/>
     </row>
-    <row r="45" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="45" spans="1:5" s="3" customFormat="1">
       <c r="A45" s="37" t="str">
         <f>IF(LEFT(B45,2)="No",0,IF(LEFT(B45,7)="Partial",0.01,IF(LEFT(B45,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2940,7 +3093,7 @@
       </c>
       <c r="E45" s="25"/>
     </row>
-    <row r="46" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="46" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A46" s="38" t="str">
         <f>IF(LEFT(B46,2)="No",0,IF(LEFT(B46,7)="Partial",0.01,IF(LEFT(B46,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2951,7 +3104,7 @@
       </c>
       <c r="E46" s="25"/>
     </row>
-    <row r="47" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="47" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A47" s="38" t="str">
         <f>IF(LEFT(B47,2)="No",0,IF(LEFT(B47,7)="Partial",0.01,IF(LEFT(B47,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2962,7 +3115,7 @@
       </c>
       <c r="E47" s="25"/>
     </row>
-    <row r="48" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="48" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A48" s="39" t="str">
         <f>IF(LEFT(B48,2)="No",0,IF(LEFT(B48,7)="Partial",0.01,IF(LEFT(B48,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2976,7 +3129,7 @@
     <row r="49" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
       <c r="C49" s="27"/>
     </row>
-    <row r="50" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="50" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A50" s="36">
         <f>IF(LEFT(B50,2)="No",0,IF(LEFT(B50,7)="Partial",0.02,IF(LEFT(B50,4)="Full",0.04,"n/a")))</f>
         <v>0</v>
@@ -2989,72 +3142,72 @@
       </c>
       <c r="E50" s="25"/>
     </row>
-    <row r="51" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="51" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A51" s="37">
         <f>IF(LEFT(B51,2)="No",-0.1,IF(LEFT(B51,7)="Partial",0,IF(LEFT(B51,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E51" s="25"/>
     </row>
-    <row r="52" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="52" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A52" s="38">
         <f>IF(LEFT(B52,2)="No",-0.1,IF(LEFT(B52,7)="Partial",0,IF(LEFT(B52,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B52" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E52" s="24"/>
     </row>
-    <row r="53" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="53" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A53" s="38">
         <f>IF(LEFT(B53,2)="No",-0.1,IF(LEFT(B53,7)="Partial",0,IF(LEFT(B53,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B53" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>52</v>
       </c>
       <c r="E53" s="24"/>
     </row>
-    <row r="54" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="54" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A54" s="38">
         <f>IF(LEFT(B54,2)="No",-0.1,IF(LEFT(B54,7)="Partial",0,IF(LEFT(B54,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E54" s="24"/>
     </row>
-    <row r="55" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="55" spans="1:5" s="3" customFormat="1" ht="31.8" thickBot="1">
       <c r="A55" s="39">
         <f>IF(LEFT(B55,2)="No",-0.1,IF(LEFT(B55,7)="Partial",0,IF(LEFT(B55,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>15</v>
       </c>
       <c r="E55" s="25"/>
     </row>
-    <row r="56" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="56" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A56" s="38" t="str">
         <f>IF(LEFT(B56,2)="No",0,IF(LEFT(B56,7)="Partial",0.01,IF(LEFT(B56,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3065,7 +3218,7 @@
       </c>
       <c r="E56" s="25"/>
     </row>
-    <row r="57" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="57" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A57" s="38" t="str">
         <f>IF(LEFT(B57,2)="No",0,IF(LEFT(B57,7)="Partial",0.01,IF(LEFT(B57,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3076,7 +3229,7 @@
       </c>
       <c r="E57" s="25"/>
     </row>
-    <row r="58" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="58" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A58" s="38" t="str">
         <f>IF(LEFT(B58,2)="No",0,IF(LEFT(B58,7)="Partial",0.01,IF(LEFT(B58,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3087,7 +3240,7 @@
       </c>
       <c r="E58" s="25"/>
     </row>
-    <row r="59" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="59" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A59" s="39" t="str">
         <f>IF(LEFT(B59,2)="No",0,IF(LEFT(B59,7)="Partial",0.01,IF(LEFT(B59,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3098,10 +3251,10 @@
       </c>
       <c r="E59" s="25"/>
     </row>
-    <row r="60" spans="1:5" ht="7.9" customHeight="1" thickBot="1">
+    <row r="60" spans="1:5" ht="7.95" customHeight="1" thickBot="1">
       <c r="E60" s="25"/>
     </row>
-    <row r="61" spans="1:5" s="50" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="61" spans="1:5" s="50" customFormat="1" ht="18.600000000000001" thickBot="1">
       <c r="A61" s="48" t="str">
         <f>IF(LEFT(B61,1)="5",0.05,IF(LEFT(B61,1)="4",0.04,IF(LEFT(B61,1)="3",0.03,IF(LEFT(B61,1)="2",0.02,IF(LEFT(B61,1)="1",0.01,IF(LEFT(B61,1)="O",0,IF(LEFT(B61,1)="L",0,"n/a")))))))</f>
         <v>n/a</v>
@@ -3112,7 +3265,7 @@
       </c>
       <c r="E61" s="51"/>
     </row>
-    <row r="62" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="62" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A62" s="37">
         <f>IF(LEFT(B62,2)="No",-0.1,IF(LEFT(B62,7)="Partial",0,IF(LEFT(B62,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -3125,20 +3278,20 @@
       </c>
       <c r="E62" s="25"/>
     </row>
-    <row r="63" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="63" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A63" s="38">
         <f>IF(LEFT(B63,2)="No",-0.1,IF(LEFT(B63,7)="Partial",0,IF(LEFT(B63,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B63" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E63" s="25"/>
     </row>
-    <row r="64" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="64" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A64" s="38">
         <f>IF(LEFT(B64,2)="No",-0.1,IF(LEFT(B64,7)="Partial",0,IF(LEFT(B64,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -3151,31 +3304,33 @@
       </c>
       <c r="E64" s="26"/>
     </row>
-    <row r="65" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="65" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A65" s="38">
         <f>IF(LEFT(B65,2)="No",-0.1,IF(LEFT(B65,7)="Partial",0,IF(LEFT(B65,4)="Full",0.02,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.02</v>
       </c>
       <c r="B65" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E65" s="26"/>
     </row>
-    <row r="66" spans="1:5" ht="16.149999999999999" customHeight="1" thickBot="1">
-      <c r="A66" s="39" t="str">
+    <row r="66" spans="1:5" ht="31.8" thickBot="1">
+      <c r="A66" s="39">
         <f>IF(LEFT(B66,2)="No",-0.1,IF(LEFT(B66,7)="Partial",0,IF(LEFT(B66,4)="Full",0.02,"n/a")))</f>
-        <v>n/a</v>
-      </c>
-      <c r="B66" s="42"/>
+        <v>0.02</v>
+      </c>
+      <c r="B66" s="42" t="s">
+        <v>79</v>
+      </c>
       <c r="C66" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E66" s="25"/>
     </row>
-    <row r="67" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="67" spans="1:5" s="3" customFormat="1">
       <c r="A67" s="37" t="str">
         <f>IF(LEFT(B67,2)="No",0,IF(LEFT(B67,7)="Partial",0.01,IF(LEFT(B67,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3186,7 +3341,7 @@
       </c>
       <c r="E67" s="25"/>
     </row>
-    <row r="68" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="68" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A68" s="38" t="str">
         <f>IF(LEFT(B68,2)="No",0,IF(LEFT(B68,7)="Partial",0.01,IF(LEFT(B68,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3197,7 +3352,7 @@
       </c>
       <c r="E68" s="25"/>
     </row>
-    <row r="69" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
+    <row r="69" spans="1:5" s="3" customFormat="1" ht="31.2">
       <c r="A69" s="38" t="str">
         <f>IF(LEFT(B69,2)="No",0,IF(LEFT(B69,7)="Partial",0.01,IF(LEFT(B69,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3208,7 +3363,7 @@
       </c>
       <c r="E69" s="25"/>
     </row>
-    <row r="70" spans="1:5" s="3" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1">
+    <row r="70" spans="1:5" s="3" customFormat="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A70" s="39" t="str">
         <f>IF(LEFT(B70,2)="No",0,IF(LEFT(B70,7)="Partial",0.01,IF(LEFT(B70,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3402,31 +3557,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9B2E6A-0D51-4D50-A1BC-AE4071052ED9}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="89.7109375" customWidth="1"/>
+    <col min="1" max="1" width="89.6640625" customWidth="1"/>
+    <col min="2" max="2" width="77.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="24" thickBot="1">
+    <row r="1" spans="1:2" ht="24" thickBot="1">
       <c r="A1" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" s="20" customFormat="1" ht="16.5" thickBot="1">
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="20" customFormat="1" ht="16.2" thickBot="1">
       <c r="A2" s="21" t="str">
         <f>IF(LEN(A3) &gt; 1000,"",IF(LEN(A3) &gt; 500,"You need more post-mortem reflection.",IF(A3&gt;0,IF(A3="If you think you have accomplished one or more bonus goals that you are worried might be overlooked, mention those here.","How did the project go? What did you learn? What could you improve?","You need A LOT MORE post-mortem reflection."),"How did the project go? What did you learn? What could you improve?")))</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="409.5" customHeight="1" thickBot="1">
+    <row r="3" spans="1:2" ht="409.5" customHeight="1" thickBot="1">
       <c r="A3" s="17" t="s">
         <v>82</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3436,52 +3598,395 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBE5BAE-5E9F-4A68-ADFA-DBB5B7061E7B}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="28" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="28"/>
-    <col min="6" max="6" width="8.85546875" style="29"/>
-    <col min="7" max="7" width="11.5703125" style="28" customWidth="1"/>
-    <col min="8" max="11" width="11.5703125" style="29" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="27.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="28"/>
+    <col min="6" max="6" width="8.88671875" style="29"/>
+    <col min="7" max="7" width="11.5546875" style="28" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.5546875" style="29" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="24" thickBot="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-    </row>
-    <row r="2" spans="1:11" ht="34.15" customHeight="1" thickBot="1">
-      <c r="A2" s="62" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+    </row>
+    <row r="2" spans="1:11" ht="34.200000000000003" customHeight="1" thickBot="1">
+      <c r="A2" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="65"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4">
+        <v>222</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4">
+        <v>144</v>
+      </c>
+      <c r="H4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5">
+        <v>160</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5">
+        <v>284</v>
+      </c>
+      <c r="H5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6">
+        <v>540</v>
+      </c>
+      <c r="D6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6">
+        <v>337</v>
+      </c>
+      <c r="H6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7">
+        <v>107</v>
+      </c>
+      <c r="D7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9">
+        <v>184</v>
+      </c>
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9">
+        <v>133</v>
+      </c>
+      <c r="H9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13">
+        <v>194</v>
+      </c>
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13">
+        <v>64</v>
+      </c>
+      <c r="H13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="H14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15">
+        <v>124</v>
+      </c>
+      <c r="D15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15">
+        <v>226</v>
+      </c>
+      <c r="H15" t="s">
+        <v>118</v>
+      </c>
+      <c r="I15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="H16" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17">
+        <v>95</v>
+      </c>
+      <c r="H17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I17">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18">
+        <v>1979084</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18">
+        <v>1199733</v>
+      </c>
+      <c r="H18" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18">
+        <v>1012673</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19">
+        <v>707</v>
+      </c>
+      <c r="D19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19">
+        <v>715</v>
+      </c>
+      <c r="H19" t="s">
+        <v>121</v>
+      </c>
+      <c r="I19">
+        <v>509</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3496,12 +4001,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6F06A3-3058-4E5E-8648-85AEA2F13214}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:C21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickBot="1">
@@ -3511,57 +4018,65 @@
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="16.5" thickBot="1">
+    <row r="2" spans="1:3" ht="16.2" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>IF(LEN(A3) &gt; 5,"","&lt;-- What lab goals had already been met at the time of this test (roughly)?")</f>
-        <v>&lt;-- What lab goals had already been met at the time of this test (roughly)?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A3" s="15"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1">
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A3" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.2" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>IF(LEN(A5) &gt; 2,"","&lt;-- What date did the playtest occur (time of day not needed)?")</f>
-        <v>&lt;-- What date did the playtest occur (time of day not needed)?</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A5" s="16"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A5" s="16">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.2" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>IF(LEN(A7) &gt; 2,"","&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?")</f>
-        <v>&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A7" s="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A7" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="16.5" thickBot="1">
+    <row r="8" spans="1:3" ht="16.2" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>IF(LEN(A9) &gt; 0,"","&lt;-- Rough total session length in minutes.")</f>
-        <v>&lt;-- Rough total session length in minutes.</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A9" s="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A9" s="15" t="s">
+        <v>86</v>
+      </c>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickBot="1">
+    <row r="10" spans="1:3" ht="16.2" thickBot="1">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -3570,79 +4085,91 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A11" s="65"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-    </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A11" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+    </row>
+    <row r="12" spans="1:3" ht="16.2" thickBot="1">
       <c r="A12" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>IF(LEN(A13)&gt;20,"","&lt;-- Relevant information about the tester (age, relationship, degree program, experience with this game/games in general, etc.)")</f>
-        <v>&lt;-- Relevant information about the tester (age, relationship, degree program, experience with this game/games in general, etc.)</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A13" s="65"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
-    </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A13" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="67"/>
+      <c r="C13" s="68"/>
+    </row>
+    <row r="14" spans="1:3" ht="16.2" thickBot="1">
       <c r="A14" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>IF(LEN(A3) &gt; 10,"","&lt;-- How was the tester measured (direct observation, survey, interview, telemetry, etc.)?")</f>
-        <v>&lt;-- How was the tester measured (direct observation, survey, interview, telemetry, etc.)?</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A15" s="65"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-    </row>
-    <row r="16" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A15" s="66" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="67"/>
+      <c r="C15" s="68"/>
+    </row>
+    <row r="16" spans="1:3" ht="16.2" thickBot="1">
       <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>IF(LEN(A17) &gt; 1000,"",IF(LEN(A17) &gt; 500,"&lt;-- You need more observational notes.",IF(A17&gt;0,"&lt;-- You need A LOT MORE observational notes.","&lt;-- What did you observe during this playtest session? (Described in full sentences, not just a list of raw notes.)")))</f>
-        <v>&lt;-- What did you observe during this playtest session? (Described in full sentences, not just a list of raw notes.)</v>
+        <v>&lt;-- You need more observational notes.</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="210" customHeight="1" thickBot="1">
-      <c r="A17" s="65"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="67"/>
-    </row>
-    <row r="18" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A17" s="66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="68"/>
+    </row>
+    <row r="18" spans="1:3" ht="16.2" thickBot="1">
       <c r="A18" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>IF(LEN(A19) &gt; 500,"",IF(LEN(A19) &gt; 250,"&lt;-- You need more findings.",IF(A19&gt;0,"&lt;-- You need A LOT MORE findings.","&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?")))</f>
-        <v>&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?</v>
+        <v>&lt;-- You need more findings.</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
-      <c r="A19" s="65"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="67"/>
-    </row>
-    <row r="20" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A19" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="67"/>
+      <c r="C19" s="68"/>
+    </row>
+    <row r="20" spans="1:3" ht="16.2" thickBot="1">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>IF(LEN(A21) &gt; 500,"",IF(LEN(A21) &gt; 250,"&lt;-- You need more recommendations.",IF(A21&gt;0,"&lt;-- You need A LOT MORE recommendations.","&lt;-- What changes would you recommend be made, and what do you think needs further research?")))</f>
-        <v>&lt;-- What changes would you recommend be made, and what do you think needs further research?</v>
+        <v>&lt;-- You need more recommendations.</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
-      <c r="A21" s="68"/>
-      <c r="B21" s="69"/>
-      <c r="C21" s="70"/>
+      <c r="A21" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="70"/>
+      <c r="C21" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3666,12 +4193,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E87B52D-2378-4812-BEF4-227AC8609A70}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:C21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickBot="1">
@@ -3681,57 +4210,65 @@
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="16.5" thickBot="1">
+    <row r="2" spans="1:3" ht="16.2" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>IF(LEN(A3) &gt; 5,"","&lt;-- What lab goals had already been met at the time of this test (roughly)?")</f>
-        <v>&lt;-- What lab goals had already been met at the time of this test (roughly)?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A3" s="15"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1">
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A3" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.2" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>IF(LEN(A5) &gt; 2,"","&lt;-- What date did the playtest occur (time of day not needed)?")</f>
-        <v>&lt;-- What date did the playtest occur (time of day not needed)?</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A5" s="16"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A5" s="16">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.2" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>IF(LEN(A7) &gt; 2,"","&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?")</f>
-        <v>&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A7" s="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A7" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="16.5" thickBot="1">
+    <row r="8" spans="1:3" ht="16.2" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>IF(LEN(A9) &gt; 0,"","&lt;-- Rough total session length in minutes.")</f>
-        <v>&lt;-- Rough total session length in minutes.</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A9" s="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A9" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickBot="1">
+    <row r="10" spans="1:3" ht="16.2" thickBot="1">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -3740,79 +4277,91 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A11" s="65"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-    </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A11" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+    </row>
+    <row r="12" spans="1:3" ht="16.2" thickBot="1">
       <c r="A12" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>IF(LEN(A13)&gt;20,"","&lt;-- Relevant information about the tester (age, relationship, degree program, experience with this game/games in general, etc.)")</f>
-        <v>&lt;-- Relevant information about the tester (age, relationship, degree program, experience with this game/games in general, etc.)</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A13" s="65"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
-    </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A13" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="67"/>
+      <c r="C13" s="68"/>
+    </row>
+    <row r="14" spans="1:3" ht="16.2" thickBot="1">
       <c r="A14" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>IF(LEN(A3) &gt; 10,"","&lt;-- How was the tester measured (direct observation, survey, interview, telemetry, etc.)?")</f>
-        <v>&lt;-- How was the tester measured (direct observation, survey, interview, telemetry, etc.)?</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A15" s="65"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-    </row>
-    <row r="16" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A15" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="67"/>
+      <c r="C15" s="68"/>
+    </row>
+    <row r="16" spans="1:3" ht="16.2" thickBot="1">
       <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>IF(LEN(A17) &gt; 1000,"",IF(LEN(A17) &gt; 500,"&lt;-- You need more observational notes.",IF(A17&gt;0,"&lt;-- You need A LOT MORE observational notes.","&lt;-- What did you observe during this playtest session? (Described in full sentences, not just a list of raw notes.)")))</f>
-        <v>&lt;-- What did you observe during this playtest session? (Described in full sentences, not just a list of raw notes.)</v>
+        <v>&lt;-- You need more observational notes.</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="210" customHeight="1" thickBot="1">
-      <c r="A17" s="65"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="67"/>
-    </row>
-    <row r="18" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A17" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="68"/>
+    </row>
+    <row r="18" spans="1:3" ht="16.2" thickBot="1">
       <c r="A18" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>IF(LEN(A19) &gt; 500,"",IF(LEN(A19) &gt; 250,"&lt;-- You need more findings.",IF(A19&gt;0,"&lt;-- You need A LOT MORE findings.","&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?")))</f>
-        <v>&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
-      <c r="A19" s="65"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="67"/>
-    </row>
-    <row r="20" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A19" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="67"/>
+      <c r="C19" s="68"/>
+    </row>
+    <row r="20" spans="1:3" ht="16.2" thickBot="1">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>IF(LEN(A21) &gt; 500,"",IF(LEN(A21) &gt; 250,"&lt;-- You need more recommendations.",IF(A21&gt;0,"&lt;-- You need A LOT MORE recommendations.","&lt;-- What changes would you recommend be made, and what do you think needs further research?")))</f>
-        <v>&lt;-- What changes would you recommend be made, and what do you think needs further research?</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
-      <c r="A21" s="68"/>
-      <c r="B21" s="69"/>
-      <c r="C21" s="70"/>
+      <c r="A21" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="70"/>
+      <c r="C21" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3823,7 +4372,7 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:C19"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{2D5A0020-17F4-42CC-B8CD-709B6D02E0E8}">
       <formula1>"Lab A Goals Met,Lab B Goals Met,Lab C Goals Met,Lab D Goals Met, Lab E Goals Met"</formula1>
     </dataValidation>
@@ -3836,12 +4385,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4A52DB-59CF-4104-8F8D-6F5B01CDFD67}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:C21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickBot="1">
@@ -3851,57 +4402,65 @@
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="16.5" thickBot="1">
+    <row r="2" spans="1:3" ht="16.2" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>IF(LEN(A3) &gt; 5,"","&lt;-- What lab goals had already been met at the time of this test (roughly)?")</f>
-        <v>&lt;-- What lab goals had already been met at the time of this test (roughly)?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A3" s="15"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1">
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A3" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.2" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>IF(LEN(A5) &gt; 2,"","&lt;-- What date did the playtest occur (time of day not needed)?")</f>
-        <v>&lt;-- What date did the playtest occur (time of day not needed)?</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A5" s="16"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A5" s="16">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.2" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>IF(LEN(A7) &gt; 2,"","&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?")</f>
-        <v>&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A7" s="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A7" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="16.5" thickBot="1">
+    <row r="8" spans="1:3" ht="16.2" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>IF(LEN(A9) &gt; 0,"","&lt;-- Rough total session length in minutes.")</f>
-        <v>&lt;-- Rough total session length in minutes.</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A9" s="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A9" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickBot="1">
+    <row r="10" spans="1:3" ht="16.2" thickBot="1">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -3910,79 +4469,91 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A11" s="65"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-    </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A11" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+    </row>
+    <row r="12" spans="1:3" ht="16.2" thickBot="1">
       <c r="A12" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>IF(LEN(A13)&gt;20,"","&lt;-- Relevant information about the tester (age, relationship, degree program, experience with this game/games in general, etc.)")</f>
-        <v>&lt;-- Relevant information about the tester (age, relationship, degree program, experience with this game/games in general, etc.)</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A13" s="65"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
-    </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A13" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="67"/>
+      <c r="C13" s="68"/>
+    </row>
+    <row r="14" spans="1:3" ht="16.2" thickBot="1">
       <c r="A14" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>IF(LEN(A3) &gt; 10,"","&lt;-- How was the tester measured (direct observation, survey, interview, telemetry, etc.)?")</f>
-        <v>&lt;-- How was the tester measured (direct observation, survey, interview, telemetry, etc.)?</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A15" s="65"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-    </row>
-    <row r="16" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A15" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="67"/>
+      <c r="C15" s="68"/>
+    </row>
+    <row r="16" spans="1:3" ht="16.2" thickBot="1">
       <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>IF(LEN(A17) &gt; 1000,"",IF(LEN(A17) &gt; 500,"&lt;-- You need more observational notes.",IF(A17&gt;0,"&lt;-- You need A LOT MORE observational notes.","&lt;-- What did you observe during this playtest session? (Described in full sentences, not just a list of raw notes.)")))</f>
-        <v>&lt;-- What did you observe during this playtest session? (Described in full sentences, not just a list of raw notes.)</v>
+        <v>&lt;-- You need more observational notes.</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="210" customHeight="1" thickBot="1">
-      <c r="A17" s="65"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="67"/>
-    </row>
-    <row r="18" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A17" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="68"/>
+    </row>
+    <row r="18" spans="1:3" ht="16.2" thickBot="1">
       <c r="A18" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>IF(LEN(A19) &gt; 500,"",IF(LEN(A19) &gt; 250,"&lt;-- You need more findings.",IF(A19&gt;0,"&lt;-- You need A LOT MORE findings.","&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?")))</f>
-        <v>&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?</v>
+        <v>&lt;-- You need more findings.</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
-      <c r="A19" s="65"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="67"/>
-    </row>
-    <row r="20" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A19" s="66" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="67"/>
+      <c r="C19" s="68"/>
+    </row>
+    <row r="20" spans="1:3" ht="16.2" thickBot="1">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>IF(LEN(A21) &gt; 500,"",IF(LEN(A21) &gt; 250,"&lt;-- You need more recommendations.",IF(A21&gt;0,"&lt;-- You need A LOT MORE recommendations.","&lt;-- What changes would you recommend be made, and what do you think needs further research?")))</f>
-        <v>&lt;-- What changes would you recommend be made, and what do you think needs further research?</v>
+        <v>&lt;-- You need more recommendations.</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
-      <c r="A21" s="68"/>
-      <c r="B21" s="69"/>
-      <c r="C21" s="70"/>
+      <c r="A21" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="70"/>
+      <c r="C21" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4006,12 +4577,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71A852-CB0D-4774-A471-FDD5A8A85644}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:C21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickBot="1">
@@ -4021,57 +4594,65 @@
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="16.5" thickBot="1">
+    <row r="2" spans="1:3" ht="16.2" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>IF(LEN(A3) &gt; 5,"","&lt;-- What lab goals had already been met at the time of this test (roughly)?")</f>
-        <v>&lt;-- What lab goals had already been met at the time of this test (roughly)?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A3" s="15"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1">
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A3" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.2" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>IF(LEN(A5) &gt; 2,"","&lt;-- What date did the playtest occur (time of day not needed)?")</f>
-        <v>&lt;-- What date did the playtest occur (time of day not needed)?</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A5" s="16"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A5" s="16">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.2" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>IF(LEN(A7) &gt; 2,"","&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?")</f>
-        <v>&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A7" s="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A7" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="16.5" thickBot="1">
+    <row r="8" spans="1:3" ht="16.2" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>IF(LEN(A9) &gt; 0,"","&lt;-- Rough total session length in minutes.")</f>
-        <v>&lt;-- Rough total session length in minutes.</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A9" s="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16.2" thickBot="1">
+      <c r="A9" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickBot="1">
+    <row r="10" spans="1:3" ht="16.2" thickBot="1">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -4080,79 +4661,91 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A11" s="65"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-    </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A11" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+    </row>
+    <row r="12" spans="1:3" ht="16.2" thickBot="1">
       <c r="A12" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>IF(LEN(A13)&gt;20,"","&lt;-- Relevant information about the tester (age, relationship, degree program, experience with this game/games in general, etc.)")</f>
-        <v>&lt;-- Relevant information about the tester (age, relationship, degree program, experience with this game/games in general, etc.)</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A13" s="65"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
-    </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A13" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="67"/>
+      <c r="C13" s="68"/>
+    </row>
+    <row r="14" spans="1:3" ht="16.2" thickBot="1">
       <c r="A14" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>IF(LEN(A3) &gt; 10,"","&lt;-- How was the tester measured (direct observation, survey, interview, telemetry, etc.)?")</f>
-        <v>&lt;-- How was the tester measured (direct observation, survey, interview, telemetry, etc.)?</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" customHeight="1" thickBot="1">
-      <c r="A15" s="65"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-    </row>
-    <row r="16" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A15" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="67"/>
+      <c r="C15" s="68"/>
+    </row>
+    <row r="16" spans="1:3" ht="16.2" thickBot="1">
       <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>IF(LEN(A17) &gt; 1000,"",IF(LEN(A17) &gt; 500,"&lt;-- You need more observational notes.",IF(A17&gt;0,"&lt;-- You need A LOT MORE observational notes.","&lt;-- What did you observe during this playtest session? (Described in full sentences, not just a list of raw notes.)")))</f>
-        <v>&lt;-- What did you observe during this playtest session? (Described in full sentences, not just a list of raw notes.)</v>
+        <v>&lt;-- You need more observational notes.</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="210" customHeight="1" thickBot="1">
-      <c r="A17" s="65"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="67"/>
-    </row>
-    <row r="18" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A17" s="66" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="68"/>
+    </row>
+    <row r="18" spans="1:3" ht="16.2" thickBot="1">
       <c r="A18" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>IF(LEN(A19) &gt; 500,"",IF(LEN(A19) &gt; 250,"&lt;-- You need more findings.",IF(A19&gt;0,"&lt;-- You need A LOT MORE findings.","&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?")))</f>
-        <v>&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?</v>
+        <v>&lt;-- You need more findings.</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
-      <c r="A19" s="65"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="67"/>
-    </row>
-    <row r="20" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A19" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="67"/>
+      <c r="C19" s="68"/>
+    </row>
+    <row r="20" spans="1:3" ht="16.2" thickBot="1">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>IF(LEN(A21) &gt; 500,"",IF(LEN(A21) &gt; 250,"&lt;-- You need more recommendations.",IF(A21&gt;0,"&lt;-- You need A LOT MORE recommendations.","&lt;-- What changes would you recommend be made, and what do you think needs further research?")))</f>
-        <v>&lt;-- What changes would you recommend be made, and what do you think needs further research?</v>
+        <v>&lt;-- You need more recommendations.</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
-      <c r="A21" s="68"/>
-      <c r="B21" s="69"/>
-      <c r="C21" s="70"/>
+      <c r="A21" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="70"/>
+      <c r="C21" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>